<commit_message>
primera version funcional conparametros
</commit_message>
<xml_diff>
--- a/m2.xlsx
+++ b/m2.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Numero</t>
   </si>
@@ -47,13 +47,34 @@
   </si>
   <si>
     <t>Prueba 10</t>
+  </si>
+  <si>
+    <t>Prueba 11</t>
+  </si>
+  <si>
+    <t>Prueba 12</t>
+  </si>
+  <si>
+    <t>Prueba 13</t>
+  </si>
+  <si>
+    <t>Prueba 14</t>
+  </si>
+  <si>
+    <t>Prueba 15</t>
+  </si>
+  <si>
+    <t>Prueba 16</t>
+  </si>
+  <si>
+    <t>Prueba 17</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -63,6 +84,7 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -78,11 +100,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
@@ -312,21 +337,19 @@
     </row>
     <row r="2">
       <c r="A2" s="2">
-        <f t="shared" ref="A2:A11" si="1">34629922521</f>
-        <v>34629922521</v>
+        <v>3.4616366188E10</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <f>34629922521</f>
         <v>34629922521</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
-        <f t="shared" si="1"/>
-        <v>34629922521</v>
+        <v>3.4616366188E10</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
@@ -334,8 +357,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2">
-        <f t="shared" si="1"/>
-        <v>34629922521</v>
+        <v>3.4616366188E10</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -343,8 +365,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2">
-        <f t="shared" si="1"/>
-        <v>34629922521</v>
+        <v>3.4616366188E10</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
@@ -352,8 +373,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2">
-        <f t="shared" si="1"/>
-        <v>34629922521</v>
+        <v>3.4616366188E10</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
@@ -361,8 +381,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2">
-        <f t="shared" si="1"/>
-        <v>34629922521</v>
+        <v>3.4616366188E10</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
@@ -370,8 +389,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2">
-        <f t="shared" si="1"/>
-        <v>34629922521</v>
+        <v>3.4616366188E10</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>8</v>
@@ -379,8 +397,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2">
-        <f t="shared" si="1"/>
-        <v>34629922521</v>
+        <v>3.4616366188E10</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
@@ -388,8 +405,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2">
-        <f t="shared" si="1"/>
-        <v>34629922521</v>
+        <v>3.4616366188E10</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>10</v>
@@ -397,11 +413,66 @@
     </row>
     <row r="11">
       <c r="A11" s="2">
-        <f t="shared" si="1"/>
-        <v>34629922521</v>
+        <v>3.4616366188E10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>3.4616366188E10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>3.4616366188E10</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>3.4616366188E10</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>3.4616366188E10</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>3.4616366188E10</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>3.4616366188E10</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
+        <v>3.4616366188E10</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>